<commit_message>
More moving of asset deemed not ready for R1.
Signed-off-by: Dockter <dockter@almuramc.com>
</commit_message>
<xml_diff>
--- a/3.0/Crop Configuration.xlsx
+++ b/3.0/Crop Configuration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="37395" windowHeight="17955" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="21630" windowHeight="13155" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Crops" sheetId="1" r:id="rId1"/>
@@ -1775,7 +1775,7 @@
   <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+      <selection activeCell="P31" sqref="P31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,7 +1812,7 @@
       <c r="A2" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="7" t="s">
         <v>81</v>
       </c>
       <c r="C2" s="11"/>
@@ -1850,7 +1850,7 @@
       <c r="A7" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>83</v>
       </c>
       <c r="C7" s="11"/>
@@ -1888,7 +1888,7 @@
       <c r="A12" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="7" t="s">
         <v>85</v>
       </c>
       <c r="C12" s="11"/>
@@ -1926,7 +1926,7 @@
       <c r="A17" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="7" t="s">
         <v>87</v>
       </c>
       <c r="C17" s="11"/>
@@ -1964,7 +1964,7 @@
       <c r="A22" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="7" t="s">
         <v>89</v>
       </c>
       <c r="C22" s="11"/>
@@ -2002,7 +2002,7 @@
       <c r="A27" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="7" t="s">
         <v>91</v>
       </c>
       <c r="C27" s="11"/>
@@ -2040,7 +2040,7 @@
       <c r="A32" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="7" t="s">
         <v>93</v>
       </c>
       <c r="C32" s="11"/>
@@ -2078,7 +2078,7 @@
       <c r="A37" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="7" t="s">
         <v>95</v>
       </c>
       <c r="C37" s="11"/>

</xml_diff>